<commit_message>
add new field [Ref] to Excels for Property, and update NFFileProcess.
add Convertion for UTF8 to GBK in NFFileProcess.
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Buff.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Buff.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19455" windowHeight="9990"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
   <si>
     <t>Id</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Cache</t>
+  </si>
+  <si>
+    <t>Ref</t>
   </si>
   <si>
     <t>Desc</t>
@@ -116,10 +119,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -136,30 +139,122 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,107 +269,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -308,25 +311,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,19 +395,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,55 +473,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,78 +491,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -541,6 +544,19 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -586,8 +602,75 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -611,21 +694,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -642,30 +710,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -674,172 +718,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -852,25 +881,31 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1262,10 +1297,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1283,71 +1318,71 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="27" spans="1:10">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" spans="1:10">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" spans="1:10">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="2" t="b">
@@ -1379,7 +1414,7 @@
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:10">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="2" t="b">
@@ -1411,7 +1446,7 @@
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="1:10">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="b">
@@ -1443,7 +1478,7 @@
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:10">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2" t="b">
@@ -1474,106 +1509,138 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="81.75" spans="1:10">
-      <c r="A7" s="9" t="s">
+    <row r="7" s="3" customFormat="1" spans="1:10">
+      <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="4" customFormat="1" ht="81.75" spans="1:10">
+      <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="C8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="D8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="E8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="10" t="s">
+      <c r="F8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="G8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="I8" s="12" t="s">
         <v>25</v>
       </c>
+      <c r="J8" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="8" s="4" customFormat="1" spans="1:10">
-      <c r="A8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="11" t="s">
+    <row r="9" s="5" customFormat="1" spans="1:10">
+      <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4">
-        <v>1</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="B9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="1" spans="1:10">
-      <c r="A9" s="4" t="s">
+    <row r="10" s="5" customFormat="1" spans="1:10">
+      <c r="A10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4">
-        <v>1</v>
-      </c>
-      <c r="I9" s="4">
-        <v>1</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:J6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A7"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:J6 B7:J7">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>